<commit_message>
Manual Clean excel column
</commit_message>
<xml_diff>
--- a/AST-Framing-Ontario/Academic Papers Trim Documentation.xlsx
+++ b/AST-Framing-Ontario/Academic Papers Trim Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\AST-Framing-Analysis-Ontario\AST-Framing-Ontario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5055726-2A5A-4D61-8E45-6FB64D4ED654}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CF7E53-D7D5-4422-8532-615D3D299DD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-285" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="379">
   <si>
     <t>Westman (2017)</t>
   </si>
@@ -1172,6 +1172,12 @@
   </si>
   <si>
     <t>7,13</t>
+  </si>
+  <si>
+    <t>Jason Manual Clean</t>
+  </si>
+  <si>
+    <t>Elise Manual Clean</t>
   </si>
 </sst>
 </file>
@@ -2717,7 +2723,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F252DF2A-79A5-4202-A951-CAC0BE693F8B}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Ligatures">
-  <location ref="I21:J25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="K21:L25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
       <items count="4">
@@ -2765,7 +2771,7 @@
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{74601E28-3FB1-40EC-AD25-E30284EB6560}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Double Coloumns (Y/N) ">
-  <location ref="I15:J19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="K15:L19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
       <items count="4">
@@ -3074,10 +3080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J234"/>
+  <dimension ref="A1:L234"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3089,15 +3095,17 @@
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="27.5703125" style="5" customWidth="1"/>
     <col min="7" max="7" width="39.7109375" style="9" customWidth="1"/>
-    <col min="8" max="8" width="46.85546875" style="5" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" customWidth="1"/>
-    <col min="10" max="10" width="29.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="46.85546875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" customWidth="1"/>
+    <col min="12" max="12" width="29.85546875" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>232</v>
       </c>
@@ -3119,14 +3127,20 @@
       <c r="G1" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>378</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>214</v>
       </c>
@@ -3149,12 +3163,12 @@
       <c r="G2" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <f>SUM(B2:B234)</f>
         <v>2845</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>213</v>
       </c>
@@ -3177,11 +3191,11 @@
       <c r="G3" s="9">
         <v>2</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>212</v>
       </c>
@@ -3204,12 +3218,12 @@
       <c r="G4" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <f>SUM(D2:D234)</f>
         <v>660</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>211</v>
       </c>
@@ -3232,11 +3246,11 @@
       <c r="G5" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>210</v>
       </c>
@@ -3259,12 +3273,12 @@
       <c r="G6" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="I6" s="2">
-        <f>I4/I2</f>
+      <c r="K6" s="2">
+        <f>K4/K2</f>
         <v>0.23198594024604569</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>209</v>
       </c>
@@ -3288,7 +3302,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>208</v>
       </c>
@@ -3311,11 +3325,11 @@
       <c r="G8" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>207</v>
       </c>
@@ -3338,14 +3352,14 @@
       <c r="G9" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="I9" s="3">
+      <c r="K9" s="3">
         <v>2.7612268518518519E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>206</v>
       </c>
@@ -3369,7 +3383,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>205</v>
       </c>
@@ -3392,11 +3406,11 @@
       <c r="G11" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>204</v>
       </c>
@@ -3419,11 +3433,11 @@
       <c r="G12" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="I12" s="3">
+      <c r="K12" s="3">
         <v>2.5300925925925929E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>203</v>
       </c>
@@ -3447,7 +3461,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>202</v>
       </c>
@@ -3471,7 +3485,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>201</v>
       </c>
@@ -3494,14 +3508,14 @@
       <c r="G15" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="K15" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L15" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>200</v>
       </c>
@@ -3524,14 +3538,14 @@
       <c r="G16" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="I16" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="J16" s="8">
+      <c r="K16" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="L16" s="8">
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>199</v>
       </c>
@@ -3554,14 +3568,14 @@
       <c r="G17" s="9">
         <v>10</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="J17" s="8">
+      <c r="K17" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="L17" s="8">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>198</v>
       </c>
@@ -3584,12 +3598,12 @@
       <c r="G18" s="9">
         <v>10</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="K18" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="J18" s="8"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>197</v>
       </c>
@@ -3612,14 +3626,14 @@
       <c r="G19" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="K19" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="J19" s="8">
+      <c r="L19" s="8">
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>196</v>
       </c>
@@ -3643,7 +3657,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>195</v>
       </c>
@@ -3666,14 +3680,14 @@
       <c r="G21" s="9">
         <v>9</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="K21" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="J21" t="s">
+      <c r="L21" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>194</v>
       </c>
@@ -3696,14 +3710,14 @@
       <c r="G22" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="I22" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="J22" s="8">
+      <c r="K22" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="L22" s="8">
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>193</v>
       </c>
@@ -3726,14 +3740,14 @@
       <c r="G23" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="I23" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="J23" s="8">
+      <c r="K23" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="L23" s="8">
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>192</v>
       </c>
@@ -3756,12 +3770,12 @@
       <c r="G24" s="9">
         <v>5</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="K24" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="J24" s="8"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L24" s="8"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>191</v>
       </c>
@@ -3784,14 +3798,14 @@
       <c r="G25" s="9">
         <v>7</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="K25" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="J25" s="8">
+      <c r="L25" s="8">
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>190</v>
       </c>
@@ -3815,7 +3829,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>189</v>
       </c>
@@ -3839,7 +3853,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>188</v>
       </c>
@@ -3863,7 +3877,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>187</v>
       </c>
@@ -3887,7 +3901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>186</v>
       </c>
@@ -3911,7 +3925,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>185</v>
       </c>
@@ -3935,7 +3949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>184</v>
       </c>
@@ -4343,7 +4357,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>168</v>
       </c>
@@ -4366,11 +4380,11 @@
       <c r="G49" s="9">
         <v>10</v>
       </c>
-      <c r="H49" s="9" t="s">
+      <c r="J49" s="9" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>167</v>
       </c>
@@ -4394,7 +4408,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>166</v>
       </c>
@@ -4418,7 +4432,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>165</v>
       </c>
@@ -4442,7 +4456,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>164</v>
       </c>
@@ -4466,7 +4480,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>163</v>
       </c>
@@ -4490,7 +4504,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>162</v>
       </c>
@@ -4514,7 +4528,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>161</v>
       </c>
@@ -4538,7 +4552,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>160</v>
       </c>
@@ -4562,7 +4576,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>159</v>
       </c>
@@ -4586,7 +4600,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>158</v>
       </c>
@@ -4610,7 +4624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>157</v>
       </c>
@@ -4634,7 +4648,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>156</v>
       </c>
@@ -4658,7 +4672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>155</v>
       </c>
@@ -4682,7 +4696,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>154</v>
       </c>
@@ -4706,7 +4720,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>153</v>
       </c>
@@ -6266,7 +6280,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>88</v>
       </c>
@@ -6290,7 +6304,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>87</v>
       </c>
@@ -6314,7 +6328,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>86</v>
       </c>
@@ -6338,7 +6352,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>85</v>
       </c>
@@ -6362,7 +6376,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>84</v>
       </c>
@@ -6386,7 +6400,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>83</v>
       </c>
@@ -6410,7 +6424,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>82</v>
       </c>
@@ -6434,7 +6448,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>81</v>
       </c>
@@ -6458,7 +6472,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>80</v>
       </c>
@@ -6482,7 +6496,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>79</v>
       </c>
@@ -6506,7 +6520,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>78</v>
       </c>
@@ -6530,7 +6544,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>77</v>
       </c>
@@ -6554,7 +6568,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>76</v>
       </c>
@@ -6577,11 +6591,11 @@
       <c r="G141" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="H141" s="10" t="s">
+      <c r="J141" s="10" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>75</v>
       </c>
@@ -6605,7 +6619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>74</v>
       </c>
@@ -6629,7 +6643,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>73</v>
       </c>
@@ -7037,7 +7051,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>56</v>
       </c>
@@ -7061,7 +7075,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>55</v>
       </c>
@@ -7085,7 +7099,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>54</v>
       </c>
@@ -7109,7 +7123,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>53</v>
       </c>
@@ -7133,7 +7147,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>52</v>
       </c>
@@ -7157,7 +7171,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>51</v>
       </c>
@@ -7181,7 +7195,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>50</v>
       </c>
@@ -7204,11 +7218,11 @@
       <c r="G167" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="H167" s="9" t="s">
+      <c r="J167" s="9" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>49</v>
       </c>
@@ -7232,7 +7246,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>48</v>
       </c>
@@ -7256,7 +7270,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>47</v>
       </c>
@@ -7280,7 +7294,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>46</v>
       </c>
@@ -7304,7 +7318,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>45</v>
       </c>
@@ -7328,7 +7342,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>44</v>
       </c>
@@ -7352,7 +7366,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>43</v>
       </c>
@@ -7376,7 +7390,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>42</v>
       </c>
@@ -7400,7 +7414,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
"Trim" to replacec "NoRef"
</commit_message>
<xml_diff>
--- a/AST-Framing-Ontario/Academic Papers Trim Documentation.xlsx
+++ b/AST-Framing-Ontario/Academic Papers Trim Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\AST-Framing-Analysis-Ontario\AST-Framing-Ontario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CF7E53-D7D5-4422-8532-615D3D299DD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34E0EA9-0618-4946-A12D-ADE720832F94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-285" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3080,7 +3080,8 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L234"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:L235"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
@@ -3140,7 +3141,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>214</v>
       </c>
@@ -3168,7 +3169,7 @@
         <v>2845</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>213</v>
       </c>
@@ -3195,7 +3196,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>212</v>
       </c>
@@ -3250,7 +3251,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>210</v>
       </c>
@@ -3302,7 +3303,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>208</v>
       </c>
@@ -3359,7 +3360,7 @@
         <v>2.7612268518518519E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>206</v>
       </c>
@@ -3410,7 +3411,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>204</v>
       </c>
@@ -3437,7 +3438,7 @@
         <v>2.5300925925925929E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>203</v>
       </c>
@@ -3461,7 +3462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>202</v>
       </c>
@@ -3515,7 +3516,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>200</v>
       </c>
@@ -3633,7 +3634,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>196</v>
       </c>
@@ -3687,7 +3688,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>194</v>
       </c>
@@ -3717,7 +3718,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>193</v>
       </c>
@@ -3775,7 +3776,7 @@
       </c>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>191</v>
       </c>
@@ -3805,7 +3806,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>190</v>
       </c>
@@ -3853,7 +3854,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>188</v>
       </c>
@@ -3925,7 +3926,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>185</v>
       </c>
@@ -4093,7 +4094,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>179</v>
       </c>
@@ -4117,7 +4118,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>178</v>
       </c>
@@ -4189,7 +4190,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>175</v>
       </c>
@@ -4213,7 +4214,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>174</v>
       </c>
@@ -4261,7 +4262,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>172</v>
       </c>
@@ -4309,7 +4310,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>170</v>
       </c>
@@ -4384,7 +4385,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>167</v>
       </c>
@@ -4408,7 +4409,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>166</v>
       </c>
@@ -4456,7 +4457,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>164</v>
       </c>
@@ -4504,7 +4505,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>162</v>
       </c>
@@ -4552,7 +4553,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>160</v>
       </c>
@@ -4576,7 +4577,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>159</v>
       </c>
@@ -4672,7 +4673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>155</v>
       </c>
@@ -4744,7 +4745,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>152</v>
       </c>
@@ -4768,7 +4769,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>151</v>
       </c>
@@ -4792,7 +4793,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>150</v>
       </c>
@@ -4816,7 +4817,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>149</v>
       </c>
@@ -4864,7 +4865,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>147</v>
       </c>
@@ -4888,7 +4889,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>146</v>
       </c>
@@ -4912,7 +4913,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>145</v>
       </c>
@@ -4936,7 +4937,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>144</v>
       </c>
@@ -4984,7 +4985,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>142</v>
       </c>
@@ -5032,7 +5033,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>140</v>
       </c>
@@ -5080,7 +5081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>138</v>
       </c>
@@ -5128,7 +5129,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>136</v>
       </c>
@@ -5152,7 +5153,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>135</v>
       </c>
@@ -5176,7 +5177,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>134</v>
       </c>
@@ -5200,7 +5201,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>133</v>
       </c>
@@ -5248,7 +5249,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>131</v>
       </c>
@@ -5296,7 +5297,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>129</v>
       </c>
@@ -5344,7 +5345,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>127</v>
       </c>
@@ -5368,7 +5369,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>126</v>
       </c>
@@ -5440,7 +5441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>123</v>
       </c>
@@ -5464,7 +5465,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>122</v>
       </c>
@@ -5488,7 +5489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>121</v>
       </c>
@@ -5512,7 +5513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>120</v>
       </c>
@@ -5560,7 +5561,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>118</v>
       </c>
@@ -5584,7 +5585,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>117</v>
       </c>
@@ -5608,7 +5609,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>116</v>
       </c>
@@ -5680,7 +5681,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>113</v>
       </c>
@@ -5704,7 +5705,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>112</v>
       </c>
@@ -5728,7 +5729,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>111</v>
       </c>
@@ -5752,7 +5753,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>110</v>
       </c>
@@ -5776,7 +5777,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>109</v>
       </c>
@@ -5944,7 +5945,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>102</v>
       </c>
@@ -5968,7 +5969,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>101</v>
       </c>
@@ -5992,7 +5993,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>100</v>
       </c>
@@ -6016,7 +6017,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>99</v>
       </c>
@@ -6040,7 +6041,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>98</v>
       </c>
@@ -6088,7 +6089,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>96</v>
       </c>
@@ -6112,7 +6113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>95</v>
       </c>
@@ -6136,7 +6137,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>94</v>
       </c>
@@ -6160,7 +6161,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>93</v>
       </c>
@@ -6184,7 +6185,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>92</v>
       </c>
@@ -6208,7 +6209,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>91</v>
       </c>
@@ -6328,7 +6329,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>86</v>
       </c>
@@ -6448,7 +6449,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>81</v>
       </c>
@@ -6472,7 +6473,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>80</v>
       </c>
@@ -6496,7 +6497,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>79</v>
       </c>
@@ -6520,7 +6521,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>78</v>
       </c>
@@ -6643,7 +6644,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>73</v>
       </c>
@@ -6739,7 +6740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>69</v>
       </c>
@@ -6763,7 +6764,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>68</v>
       </c>
@@ -6787,7 +6788,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>67</v>
       </c>
@@ -6835,7 +6836,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>65</v>
       </c>
@@ -6859,7 +6860,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>64</v>
       </c>
@@ -6883,7 +6884,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>63</v>
       </c>
@@ -6907,7 +6908,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>62</v>
       </c>
@@ -6931,7 +6932,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>61</v>
       </c>
@@ -7003,7 +7004,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>58</v>
       </c>
@@ -7051,7 +7052,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>56</v>
       </c>
@@ -7075,7 +7076,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>55</v>
       </c>
@@ -7123,7 +7124,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>53</v>
       </c>
@@ -7147,7 +7148,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>52</v>
       </c>
@@ -7171,7 +7172,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>51</v>
       </c>
@@ -7222,7 +7223,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>49</v>
       </c>
@@ -7246,7 +7247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>48</v>
       </c>
@@ -7270,7 +7271,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>47</v>
       </c>
@@ -7294,7 +7295,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>46</v>
       </c>
@@ -7342,7 +7343,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>44</v>
       </c>
@@ -7366,7 +7367,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>43</v>
       </c>
@@ -7390,7 +7391,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>42</v>
       </c>
@@ -7414,7 +7415,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>41</v>
       </c>
@@ -7438,7 +7439,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>40</v>
       </c>
@@ -7558,7 +7559,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>35</v>
       </c>
@@ -7582,7 +7583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>34</v>
       </c>
@@ -7630,7 +7631,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>32</v>
       </c>
@@ -7678,7 +7679,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>30</v>
       </c>
@@ -7702,7 +7703,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>29</v>
       </c>
@@ -7726,7 +7727,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>28</v>
       </c>
@@ -7750,7 +7751,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>27</v>
       </c>
@@ -7774,7 +7775,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>26</v>
       </c>
@@ -7822,7 +7823,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>24</v>
       </c>
@@ -7870,7 +7871,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>22</v>
       </c>
@@ -7966,7 +7967,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>18</v>
       </c>
@@ -8014,7 +8015,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>16</v>
       </c>
@@ -8038,7 +8039,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>15</v>
       </c>
@@ -8086,7 +8087,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>13</v>
       </c>
@@ -8110,7 +8111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>12</v>
       </c>
@@ -8158,7 +8159,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>10</v>
       </c>
@@ -8206,7 +8207,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>8</v>
       </c>
@@ -8230,7 +8231,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>7</v>
       </c>
@@ -8254,7 +8255,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>6</v>
       </c>
@@ -8302,7 +8303,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>4</v>
       </c>
@@ -8398,7 +8399,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>0</v>
       </c>
@@ -8422,7 +8423,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>231</v>
       </c>
@@ -8446,7 +8447,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>230</v>
       </c>
@@ -8494,7 +8495,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>228</v>
       </c>
@@ -8542,7 +8543,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>226</v>
       </c>
@@ -8614,7 +8615,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>223</v>
       </c>
@@ -8734,7 +8735,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>218</v>
       </c>
@@ -8830,8 +8831,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="235" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:F235" xr:uid="{C8FB1945-5BAC-4A3C-9D55-BBAEA124966A}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Y"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F235">
       <sortCondition ref="A1:A235"/>
     </sortState>

</xml_diff>

<commit_message>
Last update May 19th
- Applied double col function to trimmed pdf
</commit_message>
<xml_diff>
--- a/AST-Framing-Ontario/Academic Papers Trim Documentation.xlsx
+++ b/AST-Framing-Ontario/Academic Papers Trim Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\AST-Framing-Analysis-Ontario\AST-Framing-Ontario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34E0EA9-0618-4946-A12D-ADE720832F94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FE8332-1358-42F6-95AE-E47FC70D6B61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-285" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="380">
   <si>
     <t>Westman (2017)</t>
   </si>
@@ -1178,6 +1178,9 @@
   </si>
   <si>
     <t>Elise Manual Clean</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -3084,7 +3087,7 @@
   <dimension ref="A1:L235"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3096,7 +3099,7 @@
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="27.5703125" style="5" customWidth="1"/>
     <col min="7" max="7" width="39.7109375" style="9" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="24" style="9" customWidth="1"/>
     <col min="9" max="9" width="25.42578125" style="9" customWidth="1"/>
     <col min="10" max="10" width="46.85546875" style="5" customWidth="1"/>
     <col min="11" max="11" width="23.85546875" customWidth="1"/>
@@ -3301,6 +3304,9 @@
       </c>
       <c r="G7" s="9" t="s">
         <v>262</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Manual Clean Double Col Part 1
</commit_message>
<xml_diff>
--- a/AST-Framing-Ontario/Academic Papers Trim Documentation.xlsx
+++ b/AST-Framing-Ontario/Academic Papers Trim Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\AST-Framing-Analysis-Ontario\AST-Framing-Ontario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1D2A95-753A-454C-BBC4-64D15A38B543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84EC38F-DB95-4F23-831F-B227C8AF3D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12315" yWindow="2160" windowWidth="15435" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="380">
   <si>
     <t>Westman (2017)</t>
   </si>
@@ -3086,8 +3086,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H236" sqref="H236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5627,7 +5627,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>120</v>
       </c>
@@ -5651,7 +5651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>119</v>
       </c>
@@ -5675,7 +5675,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>118</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>117</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>116</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>115</v>
       </c>
@@ -5770,8 +5770,11 @@
       <c r="G102" s="9" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H102" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>114</v>
       </c>
@@ -5794,8 +5797,11 @@
       <c r="G103" s="9" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H103" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>113</v>
       </c>
@@ -5819,7 +5825,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>112</v>
       </c>
@@ -5843,7 +5849,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>111</v>
       </c>
@@ -5867,7 +5873,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>110</v>
       </c>
@@ -5891,7 +5897,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>109</v>
       </c>
@@ -5915,7 +5921,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -5938,8 +5944,11 @@
       <c r="G109" s="9" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H109" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>107</v>
       </c>
@@ -5962,8 +5971,11 @@
       <c r="G110" s="9" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H110" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>106</v>
       </c>
@@ -5986,8 +5998,11 @@
       <c r="G111" s="9" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H111" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>105</v>
       </c>
@@ -6010,8 +6025,11 @@
       <c r="G112" s="9">
         <v>10</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H112" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>104</v>
       </c>
@@ -6034,8 +6052,11 @@
       <c r="G113" s="9" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H113" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>103</v>
       </c>
@@ -6058,8 +6079,11 @@
       <c r="G114" s="9">
         <v>10</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H114" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>102</v>
       </c>
@@ -6083,7 +6107,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>101</v>
       </c>
@@ -6107,7 +6131,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>100</v>
       </c>
@@ -6131,7 +6155,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>99</v>
       </c>
@@ -6155,7 +6179,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>98</v>
       </c>
@@ -6179,7 +6203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>97</v>
       </c>
@@ -6202,8 +6226,11 @@
       <c r="G120" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H120" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>96</v>
       </c>
@@ -6227,7 +6254,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>95</v>
       </c>
@@ -6251,7 +6278,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>94</v>
       </c>
@@ -6275,7 +6302,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>93</v>
       </c>
@@ -6299,7 +6326,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>92</v>
       </c>
@@ -6323,7 +6350,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>91</v>
       </c>
@@ -6347,7 +6374,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>90</v>
       </c>
@@ -6370,8 +6397,11 @@
       <c r="G127" s="9">
         <v>7</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H127" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>89</v>
       </c>
@@ -6394,6 +6424,9 @@
       <c r="G128" s="9" t="s">
         <v>267</v>
       </c>
+      <c r="H128" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
@@ -6418,6 +6451,9 @@
       <c r="G129" s="9" t="s">
         <v>356</v>
       </c>
+      <c r="H129" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
@@ -6442,6 +6478,9 @@
       <c r="G130" s="9">
         <v>7</v>
       </c>
+      <c r="H130" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
@@ -6490,6 +6529,9 @@
       <c r="G132" s="9">
         <v>8</v>
       </c>
+      <c r="H132" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
@@ -6541,6 +6583,9 @@
       <c r="G134" s="9" t="s">
         <v>296</v>
       </c>
+      <c r="H134" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
@@ -6565,6 +6610,9 @@
       <c r="G135" s="9" t="s">
         <v>357</v>
       </c>
+      <c r="H135" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
@@ -6685,6 +6733,9 @@
       <c r="G140" s="9" t="s">
         <v>268</v>
       </c>
+      <c r="H140" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
@@ -6709,6 +6760,9 @@
       <c r="G141" s="9" t="s">
         <v>304</v>
       </c>
+      <c r="H141" s="9" t="s">
+        <v>377</v>
+      </c>
       <c r="J141" s="10" t="s">
         <v>250</v>
       </c>
@@ -6736,6 +6790,9 @@
       <c r="G142" s="9">
         <v>10</v>
       </c>
+      <c r="H142" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
@@ -6760,6 +6817,9 @@
       <c r="G143" s="9" t="s">
         <v>358</v>
       </c>
+      <c r="H143" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
@@ -6785,7 +6845,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>72</v>
       </c>
@@ -6808,8 +6868,11 @@
       <c r="G145" s="9" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H145" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>71</v>
       </c>
@@ -6832,8 +6895,11 @@
       <c r="G146" s="9" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H146" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>70</v>
       </c>
@@ -6856,8 +6922,11 @@
       <c r="G147" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H147" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>69</v>
       </c>
@@ -6881,7 +6950,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>68</v>
       </c>
@@ -6905,7 +6974,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>67</v>
       </c>
@@ -6929,7 +6998,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>66</v>
       </c>
@@ -6952,8 +7021,11 @@
       <c r="G151" s="9" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H151" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>65</v>
       </c>
@@ -6977,7 +7049,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>64</v>
       </c>
@@ -7001,7 +7073,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>63</v>
       </c>
@@ -7025,7 +7097,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>62</v>
       </c>
@@ -7049,7 +7121,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>61</v>
       </c>
@@ -7073,7 +7145,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>60</v>
       </c>
@@ -7096,8 +7168,11 @@
       <c r="G157" s="9">
         <v>6</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H157" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>59</v>
       </c>
@@ -7120,8 +7195,11 @@
       <c r="G158" s="9" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H158" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>58</v>
       </c>
@@ -7145,7 +7223,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>57</v>
       </c>
@@ -7168,6 +7246,9 @@
       <c r="G160" s="9">
         <v>11</v>
       </c>
+      <c r="H160" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
@@ -7240,6 +7321,9 @@
       <c r="G163" s="9">
         <v>7</v>
       </c>
+      <c r="H163" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
@@ -7459,6 +7543,9 @@
       <c r="G172" s="9" t="s">
         <v>362</v>
       </c>
+      <c r="H172" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
@@ -7556,7 +7643,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>40</v>
       </c>
@@ -7580,7 +7667,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>39</v>
       </c>
@@ -7603,8 +7690,11 @@
       <c r="G178" s="9" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H178" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>38</v>
       </c>
@@ -7627,8 +7717,11 @@
       <c r="G179" s="9" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H179" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>37</v>
       </c>
@@ -7651,8 +7744,11 @@
       <c r="G180" s="9" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H180" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>36</v>
       </c>
@@ -7675,8 +7771,11 @@
       <c r="G181" s="9">
         <v>9</v>
       </c>
-    </row>
-    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H181" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>35</v>
       </c>
@@ -7700,7 +7799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>34</v>
       </c>
@@ -7724,7 +7823,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>33</v>
       </c>
@@ -7747,8 +7846,11 @@
       <c r="G184" s="9" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H184" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>32</v>
       </c>
@@ -7772,7 +7874,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>31</v>
       </c>
@@ -7795,8 +7897,11 @@
       <c r="G186" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H186" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>30</v>
       </c>
@@ -7820,7 +7925,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>29</v>
       </c>
@@ -7844,7 +7949,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>28</v>
       </c>
@@ -7868,7 +7973,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>27</v>
       </c>
@@ -7892,7 +7997,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>26</v>
       </c>
@@ -7916,7 +8021,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>25</v>
       </c>
@@ -7939,8 +8044,11 @@
       <c r="G192" s="9" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H192" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>24</v>
       </c>
@@ -7964,7 +8072,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>23</v>
       </c>
@@ -7987,8 +8095,11 @@
       <c r="G194" s="9" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H194" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>22</v>
       </c>
@@ -8012,7 +8123,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>21</v>
       </c>
@@ -8035,8 +8146,11 @@
       <c r="G196" s="9" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H196" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>20</v>
       </c>
@@ -8059,8 +8173,11 @@
       <c r="G197" s="9" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H197" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>19</v>
       </c>
@@ -8083,8 +8200,11 @@
       <c r="G198" s="9">
         <v>9</v>
       </c>
-    </row>
-    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H198" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>18</v>
       </c>
@@ -8108,7 +8228,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>17</v>
       </c>
@@ -8131,8 +8251,11 @@
       <c r="G200" s="9" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H200" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>16</v>
       </c>
@@ -8156,7 +8279,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>15</v>
       </c>
@@ -8180,7 +8303,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>14</v>
       </c>
@@ -8203,8 +8326,11 @@
       <c r="G203" s="9" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H203" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>13</v>
       </c>
@@ -8228,7 +8354,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>12</v>
       </c>
@@ -8252,7 +8378,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>11</v>
       </c>
@@ -8275,8 +8401,11 @@
       <c r="G206" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H206" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>10</v>
       </c>
@@ -8300,7 +8429,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>9</v>
       </c>
@@ -8323,8 +8452,11 @@
       <c r="G208" s="9" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="209" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H208" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>8</v>
       </c>
@@ -8348,7 +8480,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="210" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>7</v>
       </c>
@@ -8372,7 +8504,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="211" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>6</v>
       </c>
@@ -8396,7 +8528,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>5</v>
       </c>
@@ -8419,8 +8551,11 @@
       <c r="G212" s="9">
         <v>8.9</v>
       </c>
-    </row>
-    <row r="213" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H212" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>4</v>
       </c>
@@ -8444,7 +8579,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>3</v>
       </c>
@@ -8467,8 +8602,11 @@
       <c r="G214" s="9" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H214" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>2</v>
       </c>
@@ -8491,8 +8629,11 @@
       <c r="G215" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H215" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>1</v>
       </c>
@@ -8515,8 +8656,11 @@
       <c r="G216" s="9" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="217" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H216" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>0</v>
       </c>
@@ -8540,7 +8684,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="218" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>231</v>
       </c>
@@ -8564,7 +8708,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="219" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>230</v>
       </c>
@@ -8588,7 +8732,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>229</v>
       </c>
@@ -8611,8 +8755,11 @@
       <c r="G220" s="9">
         <v>17</v>
       </c>
-    </row>
-    <row r="221" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H220" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>228</v>
       </c>
@@ -8636,7 +8783,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>227</v>
       </c>
@@ -8659,8 +8806,11 @@
       <c r="G222" s="9" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="223" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H222" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>226</v>
       </c>
@@ -8684,7 +8834,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>225</v>
       </c>
@@ -8707,8 +8857,11 @@
       <c r="G224" s="9" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H224" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>224</v>
       </c>
@@ -8731,8 +8884,11 @@
       <c r="G225" s="9" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="226" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H225" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>223</v>
       </c>
@@ -8756,7 +8912,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>222</v>
       </c>
@@ -8779,8 +8935,11 @@
       <c r="G227" s="9" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H227" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>221</v>
       </c>
@@ -8803,8 +8962,11 @@
       <c r="G228" s="9" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H228" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>220</v>
       </c>
@@ -8827,8 +8989,11 @@
       <c r="G229" s="9" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H229" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>219</v>
       </c>
@@ -8851,8 +9016,11 @@
       <c r="G230" s="9">
         <v>11</v>
       </c>
-    </row>
-    <row r="231" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H230" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>218</v>
       </c>
@@ -8876,7 +9044,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>217</v>
       </c>
@@ -8899,8 +9067,11 @@
       <c r="G232" s="9" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H232" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>216</v>
       </c>
@@ -8923,8 +9094,11 @@
       <c r="G233" s="9" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H233" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>215</v>
       </c>
@@ -8947,8 +9121,11 @@
       <c r="G234" s="9">
         <v>7</v>
       </c>
-    </row>
-    <row r="235" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+      <c r="H234" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:F235" xr:uid="{C8FB1945-5BAC-4A3C-9D55-BBAEA124966A}">
     <filterColumn colId="5">

</xml_diff>

<commit_message>
May 9 - 10 Changes
- Reviewed Single Column clean docs
- Fix stop words Parameters
- Updated excel documenting Academic documents
</commit_message>
<xml_diff>
--- a/AST-Framing-Ontario/Academic Papers Trim Documentation.xlsx
+++ b/AST-Framing-Ontario/Academic Papers Trim Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\AST-Framing-Analysis-Ontario\AST-Framing-Ontario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B576161-D63E-4293-8269-5C3518DF40F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42221266-B831-4D1E-9C76-C43CD87F0BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-285" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6795" yWindow="525" windowWidth="15435" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="380">
   <si>
     <t>Westman (2017)</t>
   </si>
@@ -3083,10 +3083,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L234"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:L235"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H133" sqref="H133"/>
+      <selection activeCell="H242" sqref="H242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3166,6 +3167,9 @@
       <c r="G2" s="9" t="s">
         <v>254</v>
       </c>
+      <c r="I2" s="9" t="s">
+        <v>377</v>
+      </c>
       <c r="K2">
         <f>SUM(B2:B234)</f>
         <v>2845</v>
@@ -3194,6 +3198,9 @@
       <c r="G3" s="9">
         <v>2</v>
       </c>
+      <c r="I3" s="9" t="s">
+        <v>377</v>
+      </c>
       <c r="K3" s="1" t="s">
         <v>237</v>
       </c>
@@ -3221,12 +3228,15 @@
       <c r="G4" s="9" t="s">
         <v>256</v>
       </c>
+      <c r="I4" s="9" t="s">
+        <v>377</v>
+      </c>
       <c r="K4">
         <f>SUM(D2:D234)</f>
         <v>660</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>211</v>
       </c>
@@ -3279,12 +3289,15 @@
       <c r="G6" s="9" t="s">
         <v>258</v>
       </c>
+      <c r="I6" s="9" t="s">
+        <v>377</v>
+      </c>
       <c r="K6" s="2">
         <f>K4/K2</f>
         <v>0.23198594024604569</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>209</v>
       </c>
@@ -3334,11 +3347,14 @@
       <c r="G8" s="9" t="s">
         <v>261</v>
       </c>
+      <c r="I8" s="9" t="s">
+        <v>377</v>
+      </c>
       <c r="K8" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>207</v>
       </c>
@@ -3391,8 +3407,11 @@
       <c r="G10" s="9">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I10" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>205</v>
       </c>
@@ -3445,6 +3464,9 @@
       <c r="G12" s="9" t="s">
         <v>263</v>
       </c>
+      <c r="I12" s="9" t="s">
+        <v>377</v>
+      </c>
       <c r="K12" s="3">
         <v>2.5300925925925929E-3</v>
       </c>
@@ -3472,6 +3494,9 @@
       <c r="G13" s="9">
         <v>7</v>
       </c>
+      <c r="I13" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -3496,8 +3521,11 @@
       <c r="G14" s="9" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I14" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>201</v>
       </c>
@@ -3553,6 +3581,9 @@
       <c r="G16" s="9" t="s">
         <v>266</v>
       </c>
+      <c r="I16" s="9" t="s">
+        <v>377</v>
+      </c>
       <c r="K16" s="7" t="s">
         <v>242</v>
       </c>
@@ -3560,7 +3591,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>199</v>
       </c>
@@ -3593,7 +3624,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>198</v>
       </c>
@@ -3624,7 +3655,7 @@
       </c>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>197</v>
       </c>
@@ -3680,8 +3711,11 @@
       <c r="G20" s="9" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I20" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>195</v>
       </c>
@@ -3737,6 +3771,9 @@
       <c r="G22" s="9" t="s">
         <v>269</v>
       </c>
+      <c r="I22" s="9" t="s">
+        <v>377</v>
+      </c>
       <c r="K22" s="7" t="s">
         <v>242</v>
       </c>
@@ -3767,6 +3804,9 @@
       <c r="G23" s="9" t="s">
         <v>270</v>
       </c>
+      <c r="I23" s="9" t="s">
+        <v>377</v>
+      </c>
       <c r="K23" s="7" t="s">
         <v>243</v>
       </c>
@@ -3774,7 +3814,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>192</v>
       </c>
@@ -3828,6 +3868,9 @@
       <c r="G25" s="9">
         <v>7</v>
       </c>
+      <c r="I25" s="9" t="s">
+        <v>377</v>
+      </c>
       <c r="K25" s="7" t="s">
         <v>245</v>
       </c>
@@ -3858,8 +3901,11 @@
       <c r="G26" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I26" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>189</v>
       </c>
@@ -3909,8 +3955,11 @@
       <c r="G28" s="9" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I28" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>187</v>
       </c>
@@ -3937,7 +3986,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>186</v>
       </c>
@@ -3987,8 +4036,11 @@
       <c r="G31" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I31" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>184</v>
       </c>
@@ -4012,7 +4064,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>183</v>
       </c>
@@ -4039,7 +4091,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>182</v>
       </c>
@@ -4066,7 +4118,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>181</v>
       </c>
@@ -4093,7 +4145,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>180</v>
       </c>
@@ -4120,7 +4172,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>337</v>
       </c>
@@ -4147,7 +4199,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>179</v>
       </c>
@@ -4170,8 +4222,11 @@
       <c r="G38" s="9" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>178</v>
       </c>
@@ -4194,8 +4249,11 @@
       <c r="G39" s="9" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>177</v>
       </c>
@@ -4222,7 +4280,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>176</v>
       </c>
@@ -4249,7 +4307,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>175</v>
       </c>
@@ -4273,7 +4331,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>174</v>
       </c>
@@ -4296,8 +4354,11 @@
       <c r="G43" s="9">
         <v>11</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>173</v>
       </c>
@@ -4324,7 +4385,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>172</v>
       </c>
@@ -4347,8 +4408,11 @@
       <c r="G45" s="9" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>171</v>
       </c>
@@ -4375,7 +4439,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>170</v>
       </c>
@@ -4398,8 +4462,11 @@
       <c r="G47" s="9" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>169</v>
       </c>
@@ -4426,7 +4493,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>168</v>
       </c>
@@ -4476,6 +4543,9 @@
       <c r="G50" s="9" t="s">
         <v>277</v>
       </c>
+      <c r="I50" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -4500,8 +4570,11 @@
       <c r="G51" s="9" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I51" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>165</v>
       </c>
@@ -4551,8 +4624,11 @@
       <c r="G53" s="9">
         <v>7</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I53" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>163</v>
       </c>
@@ -4602,8 +4678,11 @@
       <c r="G55" s="9" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I55" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>161</v>
       </c>
@@ -4653,6 +4732,9 @@
       <c r="G57" s="9" t="s">
         <v>280</v>
       </c>
+      <c r="I57" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -4677,8 +4759,11 @@
       <c r="G58" s="9" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I58" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>158</v>
       </c>
@@ -4705,7 +4790,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>157</v>
       </c>
@@ -4732,7 +4817,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>156</v>
       </c>
@@ -4782,8 +4867,11 @@
       <c r="G62" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I62" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>154</v>
       </c>
@@ -4810,7 +4898,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>153</v>
       </c>
@@ -4837,7 +4925,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>152</v>
       </c>
@@ -4860,8 +4948,11 @@
       <c r="G65" s="9">
         <v>11</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>151</v>
       </c>
@@ -4884,8 +4975,11 @@
       <c r="G66" s="9" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>150</v>
       </c>
@@ -4908,8 +5002,11 @@
       <c r="G67" s="9">
         <v>10</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>149</v>
       </c>
@@ -4932,8 +5029,11 @@
       <c r="G68" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>148</v>
       </c>
@@ -4960,7 +5060,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>147</v>
       </c>
@@ -4983,8 +5083,11 @@
       <c r="G70" s="9" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>146</v>
       </c>
@@ -5007,8 +5110,11 @@
       <c r="G71" s="9" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>145</v>
       </c>
@@ -5032,7 +5138,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>144</v>
       </c>
@@ -5055,8 +5161,11 @@
       <c r="G73" s="9" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>143</v>
       </c>
@@ -5083,7 +5192,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>142</v>
       </c>
@@ -5106,8 +5215,11 @@
       <c r="G75" s="9" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>141</v>
       </c>
@@ -5134,7 +5246,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>140</v>
       </c>
@@ -5157,8 +5269,11 @@
       <c r="G77" s="9">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>139</v>
       </c>
@@ -5185,7 +5300,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>138</v>
       </c>
@@ -5208,8 +5323,11 @@
       <c r="G79" s="9">
         <v>7</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>137</v>
       </c>
@@ -5236,7 +5354,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>136</v>
       </c>
@@ -5259,8 +5377,11 @@
       <c r="G81" s="9" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>135</v>
       </c>
@@ -5284,7 +5405,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>134</v>
       </c>
@@ -5307,8 +5428,11 @@
       <c r="G83" s="9" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>133</v>
       </c>
@@ -5331,8 +5455,11 @@
       <c r="G84" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>132</v>
       </c>
@@ -5359,7 +5486,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>131</v>
       </c>
@@ -5382,8 +5509,11 @@
       <c r="G86" s="9" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>130</v>
       </c>
@@ -5410,7 +5540,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>129</v>
       </c>
@@ -5433,8 +5563,11 @@
       <c r="G88" s="9" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>128</v>
       </c>
@@ -5461,7 +5594,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>127</v>
       </c>
@@ -5484,8 +5617,11 @@
       <c r="G90" s="9" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>126</v>
       </c>
@@ -5508,8 +5644,11 @@
       <c r="G91" s="9" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>125</v>
       </c>
@@ -5536,7 +5675,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>124</v>
       </c>
@@ -5563,7 +5702,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>123</v>
       </c>
@@ -5586,8 +5725,11 @@
       <c r="G94" s="9" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>122</v>
       </c>
@@ -5610,8 +5752,11 @@
       <c r="G95" s="9">
         <v>11</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>121</v>
       </c>
@@ -5634,8 +5779,11 @@
       <c r="G96" s="9">
         <v>11</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>120</v>
       </c>
@@ -5658,8 +5806,11 @@
       <c r="G97" s="9">
         <v>10</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>119</v>
       </c>
@@ -5686,7 +5837,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>118</v>
       </c>
@@ -5709,8 +5860,11 @@
       <c r="G99" s="9" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>117</v>
       </c>
@@ -5733,8 +5887,11 @@
       <c r="G100" s="9" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>116</v>
       </c>
@@ -5757,8 +5914,11 @@
       <c r="G101" s="9" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>115</v>
       </c>
@@ -5785,7 +5945,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>114</v>
       </c>
@@ -5812,7 +5972,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>113</v>
       </c>
@@ -5835,8 +5995,11 @@
       <c r="G104" s="9" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I104" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>112</v>
       </c>
@@ -5859,8 +6022,11 @@
       <c r="G105" s="9" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I105" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>111</v>
       </c>
@@ -5883,8 +6049,11 @@
       <c r="G106" s="9">
         <v>7</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I106" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>110</v>
       </c>
@@ -5907,8 +6076,11 @@
       <c r="G107" s="9">
         <v>11</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I107" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>109</v>
       </c>
@@ -5931,8 +6103,11 @@
       <c r="G108" s="9" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I108" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -5959,7 +6134,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>107</v>
       </c>
@@ -5986,7 +6161,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>106</v>
       </c>
@@ -6013,7 +6188,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>105</v>
       </c>
@@ -6040,7 +6215,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>104</v>
       </c>
@@ -6067,7 +6242,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>103</v>
       </c>
@@ -6094,7 +6269,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>102</v>
       </c>
@@ -6117,8 +6292,11 @@
       <c r="G115" s="9" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I115" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>101</v>
       </c>
@@ -6141,8 +6319,11 @@
       <c r="G116" s="9" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I116" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>100</v>
       </c>
@@ -6165,8 +6346,11 @@
       <c r="G117" s="9">
         <v>9</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I117" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>99</v>
       </c>
@@ -6189,8 +6373,11 @@
       <c r="G118" s="9">
         <v>13</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I118" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>98</v>
       </c>
@@ -6213,8 +6400,11 @@
       <c r="G119" s="9">
         <v>9</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I119" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>97</v>
       </c>
@@ -6241,7 +6431,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>96</v>
       </c>
@@ -6264,8 +6454,11 @@
       <c r="G121" s="9">
         <v>7</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I121" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>95</v>
       </c>
@@ -6288,8 +6481,11 @@
       <c r="G122" s="9">
         <v>9</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I122" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>94</v>
       </c>
@@ -6312,8 +6508,11 @@
       <c r="G123" s="9" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I123" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>93</v>
       </c>
@@ -6336,8 +6535,11 @@
       <c r="G124" s="9" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I124" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>92</v>
       </c>
@@ -6360,8 +6562,11 @@
       <c r="G125" s="9" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I125" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>91</v>
       </c>
@@ -6384,8 +6589,11 @@
       <c r="G126" s="9" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I126" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>90</v>
       </c>
@@ -6412,7 +6620,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>89</v>
       </c>
@@ -6439,7 +6647,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>88</v>
       </c>
@@ -6466,7 +6674,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>87</v>
       </c>
@@ -6516,8 +6724,11 @@
       <c r="G131" s="9" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I131" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>85</v>
       </c>
@@ -6544,7 +6755,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>84</v>
       </c>
@@ -6571,7 +6782,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>83</v>
       </c>
@@ -6598,7 +6809,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>82</v>
       </c>
@@ -6648,6 +6859,9 @@
       <c r="G136" s="9" t="s">
         <v>259</v>
       </c>
+      <c r="I136" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
@@ -6672,6 +6886,9 @@
       <c r="G137" s="9" t="s">
         <v>296</v>
       </c>
+      <c r="I137" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
@@ -6696,6 +6913,9 @@
       <c r="G138" s="9" t="s">
         <v>305</v>
       </c>
+      <c r="I138" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
@@ -6720,8 +6940,11 @@
       <c r="G139" s="9" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I139" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>77</v>
       </c>
@@ -6748,7 +6971,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>76</v>
       </c>
@@ -6778,7 +7001,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>75</v>
       </c>
@@ -6805,7 +7028,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>74</v>
       </c>
@@ -6855,8 +7078,11 @@
       <c r="G144" s="9" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I144" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>72</v>
       </c>
@@ -6883,7 +7109,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>71</v>
       </c>
@@ -6910,7 +7136,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>70</v>
       </c>
@@ -6937,7 +7163,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>69</v>
       </c>
@@ -6960,8 +7186,11 @@
       <c r="G148" s="9" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I148" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>68</v>
       </c>
@@ -6984,8 +7213,11 @@
       <c r="G149" s="9" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I149" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>67</v>
       </c>
@@ -7008,8 +7240,11 @@
       <c r="G150" s="9" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I150" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>66</v>
       </c>
@@ -7036,7 +7271,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>65</v>
       </c>
@@ -7059,8 +7294,11 @@
       <c r="G152" s="9" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I152" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>64</v>
       </c>
@@ -7083,8 +7321,11 @@
       <c r="G153" s="9" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I153" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>63</v>
       </c>
@@ -7107,8 +7348,11 @@
       <c r="G154" s="9" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I154" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>62</v>
       </c>
@@ -7131,8 +7375,11 @@
       <c r="G155" s="9" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I155" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>61</v>
       </c>
@@ -7155,8 +7402,11 @@
       <c r="G156" s="9" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I156" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>60</v>
       </c>
@@ -7183,7 +7433,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>59</v>
       </c>
@@ -7210,7 +7460,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>58</v>
       </c>
@@ -7233,8 +7483,11 @@
       <c r="G159" s="9" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I159" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>57</v>
       </c>
@@ -7284,6 +7537,9 @@
       <c r="G161" s="9" t="s">
         <v>316</v>
       </c>
+      <c r="I161" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
@@ -7308,8 +7564,11 @@
       <c r="G162" s="9" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I162" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>54</v>
       </c>
@@ -7359,6 +7618,9 @@
       <c r="G164" s="9" t="s">
         <v>317</v>
       </c>
+      <c r="I164" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
@@ -7383,6 +7645,9 @@
       <c r="G165" s="9" t="s">
         <v>307</v>
       </c>
+      <c r="I165" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
@@ -7407,8 +7672,11 @@
       <c r="G166" s="9" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I166" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>50</v>
       </c>
@@ -7458,6 +7726,9 @@
       <c r="G168" s="9">
         <v>8</v>
       </c>
+      <c r="I168" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
@@ -7482,6 +7753,9 @@
       <c r="G169" s="9" t="s">
         <v>318</v>
       </c>
+      <c r="I169" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
@@ -7506,6 +7780,9 @@
       <c r="G170" s="9">
         <v>17</v>
       </c>
+      <c r="I170" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
@@ -7530,8 +7807,11 @@
       <c r="G171" s="9" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I171" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>45</v>
       </c>
@@ -7581,6 +7861,9 @@
       <c r="G173" s="9">
         <v>7</v>
       </c>
+      <c r="I173" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
@@ -7605,6 +7888,9 @@
       <c r="G174" s="9" t="s">
         <v>320</v>
       </c>
+      <c r="I174" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
@@ -7629,6 +7915,9 @@
       <c r="G175" s="9" t="s">
         <v>265</v>
       </c>
+      <c r="I175" s="9" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
@@ -7654,7 +7943,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>40</v>
       </c>
@@ -7677,8 +7966,11 @@
       <c r="G177" s="9" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I177" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>39</v>
       </c>
@@ -7705,7 +7997,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>38</v>
       </c>
@@ -7732,7 +8024,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>37</v>
       </c>
@@ -7759,7 +8051,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>36</v>
       </c>
@@ -7786,7 +8078,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>35</v>
       </c>
@@ -7809,8 +8101,11 @@
       <c r="G182" s="9">
         <v>10</v>
       </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I182" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>34</v>
       </c>
@@ -7833,8 +8128,11 @@
       <c r="G183" s="9">
         <v>13</v>
       </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I183" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>33</v>
       </c>
@@ -7861,7 +8159,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>32</v>
       </c>
@@ -7884,8 +8182,11 @@
       <c r="G185" s="9" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I185" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>31</v>
       </c>
@@ -7912,7 +8213,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>30</v>
       </c>
@@ -7935,8 +8236,11 @@
       <c r="G187" s="9" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I187" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>29</v>
       </c>
@@ -7959,8 +8263,11 @@
       <c r="G188" s="9" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I188" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>28</v>
       </c>
@@ -7983,8 +8290,11 @@
       <c r="G189" s="9" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I189" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>27</v>
       </c>
@@ -8007,8 +8317,11 @@
       <c r="G190" s="9" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I190" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>26</v>
       </c>
@@ -8031,8 +8344,11 @@
       <c r="G191" s="9" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I191" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>25</v>
       </c>
@@ -8059,7 +8375,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>24</v>
       </c>
@@ -8082,8 +8398,11 @@
       <c r="G193" s="9" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I193" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>23</v>
       </c>
@@ -8110,7 +8429,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>22</v>
       </c>
@@ -8133,8 +8452,11 @@
       <c r="G195" s="9" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I195" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>21</v>
       </c>
@@ -8161,7 +8483,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>20</v>
       </c>
@@ -8188,7 +8510,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>19</v>
       </c>
@@ -8215,7 +8537,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>18</v>
       </c>
@@ -8238,8 +8560,11 @@
       <c r="G199" s="9">
         <v>10</v>
       </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I199" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>17</v>
       </c>
@@ -8266,7 +8591,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>16</v>
       </c>
@@ -8289,8 +8614,11 @@
       <c r="G201" s="9" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I201" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>15</v>
       </c>
@@ -8313,8 +8641,11 @@
       <c r="G202" s="9" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I202" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>14</v>
       </c>
@@ -8341,7 +8672,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>13</v>
       </c>
@@ -8364,8 +8695,11 @@
       <c r="G204" s="9">
         <v>9</v>
       </c>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I204" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>12</v>
       </c>
@@ -8388,8 +8722,11 @@
       <c r="G205" s="9" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I205" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>11</v>
       </c>
@@ -8416,7 +8753,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>10</v>
       </c>
@@ -8439,8 +8776,11 @@
       <c r="G207" s="9">
         <v>11</v>
       </c>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I207" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>9</v>
       </c>
@@ -8467,7 +8807,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>8</v>
       </c>
@@ -8490,8 +8830,11 @@
       <c r="G209" s="9" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I209" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>7</v>
       </c>
@@ -8514,8 +8857,11 @@
       <c r="G210" s="9" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I210" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>6</v>
       </c>
@@ -8538,8 +8884,11 @@
       <c r="G211" s="9" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I211" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>5</v>
       </c>
@@ -8566,7 +8915,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>4</v>
       </c>
@@ -8589,8 +8938,11 @@
       <c r="G213" s="9">
         <v>6</v>
       </c>
-    </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I213" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>3</v>
       </c>
@@ -8617,7 +8969,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>2</v>
       </c>
@@ -8644,7 +8996,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>1</v>
       </c>
@@ -8671,7 +9023,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>0</v>
       </c>
@@ -8694,8 +9046,11 @@
       <c r="G217" s="9" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I217" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>231</v>
       </c>
@@ -8718,8 +9073,11 @@
       <c r="G218" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I218" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>230</v>
       </c>
@@ -8742,8 +9100,11 @@
       <c r="G219" s="9" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I219" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>229</v>
       </c>
@@ -8770,7 +9131,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>228</v>
       </c>
@@ -8793,8 +9154,11 @@
       <c r="G221" s="9" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I221" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>227</v>
       </c>
@@ -8821,7 +9185,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>226</v>
       </c>
@@ -8844,8 +9208,11 @@
       <c r="G223" s="9" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I223" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>225</v>
       </c>
@@ -8872,7 +9239,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>224</v>
       </c>
@@ -8899,7 +9266,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>223</v>
       </c>
@@ -8922,8 +9289,11 @@
       <c r="G226" s="9" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I226" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>222</v>
       </c>
@@ -8950,7 +9320,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>221</v>
       </c>
@@ -8977,7 +9347,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>220</v>
       </c>
@@ -9004,7 +9374,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>219</v>
       </c>
@@ -9031,7 +9401,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>218</v>
       </c>
@@ -9054,8 +9424,11 @@
       <c r="G231" s="9" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I231" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>217</v>
       </c>
@@ -9082,7 +9455,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>216</v>
       </c>
@@ -9109,7 +9482,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>215</v>
       </c>
@@ -9136,8 +9509,14 @@
         <v>377</v>
       </c>
     </row>
+    <row r="235" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:F235" xr:uid="{C8FB1945-5BAC-4A3C-9D55-BBAEA124966A}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="N"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F235">
       <sortCondition ref="A1:A235"/>
     </sortState>

</xml_diff>